<commit_message>
Lisasin Courses lehe ja muutsin Courses ja Students kaustas kõigil scaffoldedmudeli itemitel namespaceid ja modelid ära, sest VS ei leidnud üles või olid topelt meetodid.
</commit_message>
<xml_diff>
--- a/Homework1-3/Time recording log.xlsx
+++ b/Homework1-3/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Katse1\Homework1-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A25811C-A4F3-44D9-A825-1223A95D4C4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DADA66C-C2C6-488A-91C9-B45DAA414649}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Kodutöö 2</t>
+  </si>
+  <si>
+    <t>minutes</t>
   </si>
 </sst>
 </file>
@@ -1240,9 +1243,13 @@
       <c r="C15" s="8">
         <v>0.47222222222222227</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="32">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>160</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1254,12 +1261,18 @@
       <c r="A16" s="9">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="7">
+        <v>43870</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.38680555555555557</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -1302,9 +1315,11 @@
       <c r="E19" s="36"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>597</v>
-      </c>
-      <c r="G19" s="28"/>
+        <v>757</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29"/>
@@ -1329,7 +1344,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1683,7 +1698,9 @@
         <f>SUM(F7:F18)</f>
         <v>920</v>
       </c>
-      <c r="G19" s="28"/>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29"/>

</xml_diff>

<commit_message>
Commit enne kodutöö 3 alustamist
</commit_message>
<xml_diff>
--- a/Homework1-3/Time recording log.xlsx
+++ b/Homework1-3/Time recording log.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Katse1\Homework1-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC4CC20-F2C4-4DB5-96C1-401ADD3F6A28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139ABD1A-291C-4608-9C4F-74745BDB92FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nädal 2" sheetId="3" r:id="rId1"/>
-    <sheet name="Nädal 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Nädal 3" sheetId="5" r:id="rId1"/>
+    <sheet name="Nädal 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Nädal 1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -140,6 +141,9 @@
   </si>
   <si>
     <t>minutes</t>
+  </si>
+  <si>
+    <t>Razor page, MVC mõisted</t>
   </si>
 </sst>
 </file>
@@ -931,11 +935,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8DD912-1C37-45A7-B4D1-E4B8ABC30324}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="46">
-        <v>43863</v>
+        <v>43877</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
@@ -1045,22 +1049,12 @@
       <c r="A7" s="17">
         <v>1</v>
       </c>
-      <c r="B7" s="18">
-        <v>43865</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0.86875000000000002</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0.88611111111111107</v>
-      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="21">
-        <v>30</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
@@ -1069,22 +1063,12 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="18">
-        <v>43865</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.90972222222222221</v>
-      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="5">
-        <v>30</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
@@ -1093,22 +1077,12 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="7">
-        <v>43866</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.81944444444444453</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="5">
-        <v>48</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1117,22 +1091,12 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7">
-        <v>43866</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.89444444444444438</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.91666666666666663</v>
-      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="5">
-        <v>30</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="31"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -1141,22 +1105,12 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7">
-        <v>43867</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.46875</v>
-      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="5">
-        <v>195</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1165,22 +1119,12 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7">
-        <v>43867</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.56944444444444442</v>
-      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="5">
-        <v>85</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -1189,22 +1133,12 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7">
-        <v>43867</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.67986111111111114</v>
-      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="5">
-        <v>89</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -1213,22 +1147,12 @@
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="7">
-        <v>43868</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.91666666666666663</v>
-      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="5">
-        <v>90</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1237,22 +1161,12 @@
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7">
-        <v>43869</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="D15" s="32">
-        <v>0.58333333333333337</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="5">
-        <v>160</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -1261,22 +1175,12 @@
       <c r="A16" s="9">
         <v>10</v>
       </c>
-      <c r="B16" s="7">
-        <v>43870</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0.38680555555555557</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0.54861111111111105</v>
-      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="5">
-        <v>230</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -1319,7 +1223,7 @@
       <c r="E19" s="36"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>987</v>
+        <v>0</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1344,11 +1248,434 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="46">
+        <v>43870</v>
+      </c>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43865</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <v>30</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
+        <v>43865</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <v>30</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43866</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>48</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
+        <v>43866</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.89444444444444438</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <v>30</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>195</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <v>85</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7">
+        <v>43867</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.67986111111111114</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <v>89</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7">
+        <v>43868</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <v>90</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7">
+        <v>43869</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <v>160</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7">
+        <v>43870</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <v>230</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7">
+        <v>43870</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <v>25</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>1012</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G4" sqref="G4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Mudelid course, student ja enrollment lisatud, kaust Data
</commit_message>
<xml_diff>
--- a/Homework1-3/Time recording log.xlsx
+++ b/Homework1-3/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Katse1\Homework1-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139ABD1A-291C-4608-9C4F-74745BDB92FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442C8FAA-0284-4C9D-9F6B-9EFE9D5131CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Razor page, MVC mõisted</t>
+  </si>
+  <si>
+    <t>Kodutöö 3</t>
   </si>
 </sst>
 </file>
@@ -939,7 +942,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1049,12 +1052,18 @@
       <c r="A7" s="17">
         <v>1</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="18">
+        <v>43876</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>

</xml_diff>

<commit_message>
coursescontroller lisatud, courses page ei tööta ei leia üles "department"it
</commit_message>
<xml_diff>
--- a/Homework1-3/Time recording log.xlsx
+++ b/Homework1-3/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Katse1\Homework1-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606FF18A-F396-4D98-ACB0-A6280C3867A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0323962-AFB9-48BC-B71E-E751A52C3C36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Kodutöö 3</t>
+  </si>
+  <si>
+    <t>Kodutöö 3, jamamine migratsioonidega</t>
   </si>
 </sst>
 </file>
@@ -942,7 +945,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,11 +1081,13 @@
       <c r="C8" s="8">
         <v>0.75</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8">
+        <v>0.90277777777777779</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
       <c r="G8" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1092,12 +1097,18 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.4513888888888889</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>

</xml_diff>

<commit_message>
code update ja time log
</commit_message>
<xml_diff>
--- a/Homework1-3/Time recording log.xlsx
+++ b/Homework1-3/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Katse1\Homework1-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0323962-AFB9-48BC-B71E-E751A52C3C36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1969522C-3A22-48C2-B3ED-76C675BA8F8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Kodutöö 3, jamamine migratsioonidega</t>
+  </si>
+  <si>
+    <t>Jamasin tükk aega DB ja migratsioonidega</t>
   </si>
 </sst>
 </file>
@@ -945,7 +948,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,13 +1106,17 @@
       <c r="C9" s="8">
         <v>0.4513888888888889</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>

</xml_diff>

<commit_message>
Commit enne inheritance tegemist
</commit_message>
<xml_diff>
--- a/Homework1-3/Time recording log.xlsx
+++ b/Homework1-3/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Katse1\Homework1-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1969522C-3A22-48C2-B3ED-76C675BA8F8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A49890-DAC1-4BA5-A758-E78B09E15BA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -948,7 +948,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,11 +1125,15 @@
         <v>4</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H10" s="31"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>

</xml_diff>